<commit_message>
Sea creature refactoring done
</commit_message>
<xml_diff>
--- a/sea_creature_pulse/vals.xlsx
+++ b/sea_creature_pulse/vals.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8196"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8196" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Blueaug</t>
+  </si>
+  <si>
+    <t>Redval</t>
+  </si>
+  <si>
+    <t>Blueval1</t>
+  </si>
+  <si>
+    <t>Blueval2</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,7 +390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -973,4 +987,169 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>(C2*2)+50 -A$2</f>
+        <v>51</v>
+      </c>
+      <c r="E2">
+        <f>(C2*2)+50 -A$3</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D11" si="0">(C3*2)+50 -A$2</f>
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E11" si="1">(C3*2)+50 -A$3</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <f>(C7*2)+50 +A$2</f>
+        <v>61</v>
+      </c>
+      <c r="E7">
+        <f>(C7*2)+50 +A$3</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:D11" si="2">(C8*2)+50 +A$2</f>
+        <v>59</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:E11" si="3">(C8*2)+50 +A$3</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>